<commit_message>
adding .xlsx files to git ignore for any additional working sheets in the directory data lookups now presents the stats with text read from "unit_stats" mod_lookup.py now includes character information adding baseline mod optimizer that reads from the mod-weights.xlsx file adjusting mod thresholds to decimal rather than percentages updating dependencies and adding openpyxl
</commit_message>
<xml_diff>
--- a/mod-weights.xlsx
+++ b/mod-weights.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ardav\Documents\python\swgoh-helper\swgoh-stat-calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ardav\Documents\python\swgoh-helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5208EAEF-1F55-4609-A444-6BFBD32E8C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9CD432-9F06-4803-A2A5-FBF5AE6477DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9CB1516-F057-4BCA-9F47-2CABFCCF5ECD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Char Mod Stat Weights" sheetId="1" r:id="rId1"/>
+    <sheet name="Recommendations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -663,27 +664,6 @@
     <t>(10, 130, 7)</t>
   </si>
   <si>
-    <t>(10, 75%, 7)</t>
-  </si>
-  <si>
-    <t>(10,  42%, 7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(10,  45%, 7) </t>
-  </si>
-  <si>
-    <t>(9, 17%, 7)</t>
-  </si>
-  <si>
-    <t>(10,  42%, 9)</t>
-  </si>
-  <si>
-    <t>(10, 85%, 7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(10,  35%, 9) </t>
-  </si>
-  <si>
     <t>(10, 72, 7)</t>
   </si>
   <si>
@@ -693,31 +673,52 @@
     <t>(10, 116, 8)</t>
   </si>
   <si>
-    <t>(10, 25.5%, 9)</t>
-  </si>
-  <si>
     <t>(10, 61, 8)</t>
   </si>
   <si>
-    <t>(10, 15%, 7)</t>
-  </si>
-  <si>
-    <t>(10,  42%, 8)</t>
-  </si>
-  <si>
-    <t>(10,  42%, 6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(10,  25%, 6) </t>
-  </si>
-  <si>
-    <t>(10,  30%, 0)</t>
-  </si>
-  <si>
     <t>Geonosian Soldier</t>
   </si>
   <si>
-    <t>(10, 45%, 8)</t>
+    <t>(10, 0.75, 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10, 0.45, 7) </t>
+  </si>
+  <si>
+    <t>(10, 0.45, 8)</t>
+  </si>
+  <si>
+    <t>(9, 0.17, 7)</t>
+  </si>
+  <si>
+    <t>(10, 0.85, 7)</t>
+  </si>
+  <si>
+    <t>(10, 0.42, 7)</t>
+  </si>
+  <si>
+    <t>(10, 0.42, 9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10, 0.35, 9) </t>
+  </si>
+  <si>
+    <t>(10, 0.15, 7)</t>
+  </si>
+  <si>
+    <t>(10, 0.42, 6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10, 0.25, 6) </t>
+  </si>
+  <si>
+    <t>(10, 0.42, 8)</t>
+  </si>
+  <si>
+    <t>(10, 0.30, 0)</t>
+  </si>
+  <si>
+    <t>(10, 0.255, 9)</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1074,8 @@
   <dimension ref="A1:L198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1139,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -1161,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1204,10 +1205,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="G5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H5">
         <v>9</v>
@@ -1255,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1295,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="K10">
         <v>8</v>
@@ -1315,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -1372,7 +1373,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1380,13 +1381,13 @@
         <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E15" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -1403,7 +1404,7 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="J16">
         <v>10</v>
@@ -1420,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I17">
         <v>10</v>
@@ -1502,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1547,7 +1548,7 @@
         <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F25">
         <v>9</v>
@@ -1570,7 +1571,7 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -1672,7 +1673,7 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F32">
         <v>9</v>
@@ -1728,13 +1729,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F36">
         <v>8</v>
@@ -1824,7 +1825,7 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -1841,7 +1842,7 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -2015,7 +2016,7 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D55">
         <v>8</v>
@@ -2029,7 +2030,7 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H56">
         <v>7</v>
@@ -2071,224 +2072,221 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="B59">
         <v>10</v>
       </c>
-      <c r="C59">
-        <v>8</v>
-      </c>
-      <c r="D59">
+      <c r="E59">
         <v>9</v>
       </c>
       <c r="K59">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>190</v>
+        <v>77</v>
       </c>
       <c r="B60">
         <v>9</v>
       </c>
       <c r="C60">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D60">
-        <v>9</v>
-      </c>
-      <c r="L60">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="K60">
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
-      </c>
-      <c r="F61">
-        <v>10</v>
-      </c>
-      <c r="I61">
-        <v>10</v>
-      </c>
-      <c r="J61">
+        <v>190</v>
+      </c>
+      <c r="B61">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61">
+        <v>9</v>
+      </c>
+      <c r="L61">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62">
-        <v>10</v>
-      </c>
-      <c r="H62">
-        <v>9</v>
+        <v>124</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
       </c>
       <c r="I62">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="J62">
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>10</v>
       </c>
-      <c r="E63">
-        <v>10</v>
-      </c>
-      <c r="F63">
+      <c r="H63">
+        <v>9</v>
+      </c>
+      <c r="I63">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>17</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
       </c>
       <c r="C64">
         <v>10</v>
       </c>
-      <c r="D64">
-        <v>8</v>
-      </c>
       <c r="E64">
         <v>10</v>
       </c>
-      <c r="H64">
+      <c r="F64">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>173</v>
-      </c>
-      <c r="B65">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="C65">
         <v>10</v>
       </c>
       <c r="D65">
-        <v>9</v>
-      </c>
-      <c r="E65" t="s">
-        <v>213</v>
-      </c>
-      <c r="F65">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+      <c r="H65">
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B66">
         <v>9</v>
       </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
       <c r="D66">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>220</v>
+      </c>
+      <c r="F66">
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="B67">
         <v>9</v>
       </c>
-      <c r="C67">
-        <v>10</v>
-      </c>
       <c r="D67">
-        <v>9</v>
-      </c>
-      <c r="E67" t="s">
-        <v>213</v>
-      </c>
-      <c r="H67">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>217</v>
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>220</v>
       </c>
       <c r="H68">
         <v>8</v>
-      </c>
-      <c r="K68">
-        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>154</v>
-      </c>
-      <c r="B69">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>210</v>
+      </c>
+      <c r="H69">
+        <v>8</v>
       </c>
       <c r="K69">
-        <v>8</v>
-      </c>
-      <c r="L69">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="B70">
-        <v>10</v>
-      </c>
-      <c r="F70">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="K70">
+        <v>8</v>
+      </c>
+      <c r="L70">
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71">
-        <v>10</v>
-      </c>
-      <c r="D71">
-        <v>9</v>
-      </c>
-      <c r="E71" t="s">
-        <v>213</v>
+        <v>20</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="F71">
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>161</v>
-      </c>
-      <c r="B72">
-        <v>8</v>
-      </c>
-      <c r="E72">
-        <v>10</v>
-      </c>
-      <c r="H72">
-        <v>8</v>
-      </c>
-      <c r="J72">
-        <v>9</v>
+        <v>123</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -2296,22 +2294,25 @@
       <c r="E73">
         <v>10</v>
       </c>
-      <c r="F73">
+      <c r="H73">
+        <v>8</v>
+      </c>
+      <c r="J73">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="B74">
-        <v>10</v>
-      </c>
-      <c r="D74">
-        <v>9</v>
-      </c>
-      <c r="K74">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="E74">
+        <v>10</v>
+      </c>
+      <c r="F74">
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -2322,7 +2323,7 @@
         <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E75">
         <v>9</v>
@@ -2407,7 +2408,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K80">
         <v>8</v>
@@ -2438,7 +2439,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -2494,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F86">
         <v>9</v>
@@ -2550,7 +2551,7 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F90">
         <v>10</v>
@@ -2782,7 +2783,7 @@
         <v>8</v>
       </c>
       <c r="E110" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -3776,5 +3777,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4412CC32-510A-4B7F-BB4F-41DE577A0E77}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>